<commit_message>
Eq L now works too
</commit_message>
<xml_diff>
--- a/Copy of Pipesize - odemceny s komenty.xlsx
+++ b/Copy of Pipesize - odemceny s komenty.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CVUT\4. semestr\KAJ\Semestralka\kaj-semestralni-prace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F7AF0A9-CBF6-49FE-8BCC-EEDC33D8BF27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F0AA20-79A7-48D6-A82A-6CA5B1928A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P" sheetId="1" r:id="rId1"/>
@@ -29,14 +29,12 @@
     <sheet name="Sheet15" sheetId="14" r:id="rId14"/>
     <sheet name="Sheet16" sheetId="15" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -232,7 +230,7 @@
     <t>Uses Darcy Equ'n for Turbulent flow</t>
   </si>
   <si>
-    <t>hg BMS</t>
+    <t>Hg BMS</t>
   </si>
 </sst>
 </file>
@@ -690,7 +688,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -723,12 +721,6 @@
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -845,9 +837,33 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -931,7 +947,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1254,415 +1270,415 @@
   <dimension ref="A1:U39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="X18" sqref="X18"/>
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="4" width="2.90625" customWidth="1"/>
+    <col min="2" max="4" width="2.85546875" customWidth="1"/>
     <col min="5" max="5" width="3" customWidth="1"/>
-    <col min="6" max="6" width="3.54296875" customWidth="1"/>
-    <col min="7" max="8" width="3.08984375" customWidth="1"/>
-    <col min="9" max="9" width="3.36328125" customWidth="1"/>
+    <col min="6" max="6" width="3.5703125" customWidth="1"/>
+    <col min="7" max="8" width="3.140625" customWidth="1"/>
+    <col min="9" max="9" width="3.42578125" customWidth="1"/>
     <col min="10" max="17" width="4" customWidth="1"/>
     <col min="18" max="18" width="5" customWidth="1"/>
-    <col min="19" max="19" width="4.453125" customWidth="1"/>
-    <col min="20" max="20" width="3.54296875" customWidth="1"/>
-    <col min="21" max="21" width="1.08984375" customWidth="1"/>
+    <col min="19" max="19" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.42578125" customWidth="1"/>
+    <col min="21" max="21" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:21" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="32" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="25"/>
+      <c r="J1" s="23"/>
       <c r="K1" s="6"/>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="28"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="30"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="M1" s="26"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="28"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="76">
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="74">
         <v>65</v>
       </c>
-      <c r="J2" s="77"/>
+      <c r="J2" s="75"/>
       <c r="K2" s="6"/>
-      <c r="L2" s="33" t="s">
+      <c r="L2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="39">
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="37">
         <f>(I3/1000)/(3.14159*(S15/2000)^2)</f>
         <v>0.56727138346870387</v>
       </c>
-      <c r="S2" s="25"/>
+      <c r="S2" s="23"/>
       <c r="T2" s="6"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="76">
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="74">
         <v>2</v>
       </c>
-      <c r="J3" s="77"/>
+      <c r="J3" s="75"/>
       <c r="K3" s="6"/>
-      <c r="L3" s="33" t="s">
+      <c r="L3" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="34"/>
-      <c r="N3" s="34"/>
-      <c r="O3" s="34"/>
-      <c r="P3" s="34"/>
-      <c r="Q3" s="38"/>
-      <c r="R3" s="40">
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="36"/>
+      <c r="R3" s="38">
         <f>IF(J13&lt;2300,data!B25,IF(J13&lt;3500,data!B27,data!B29))</f>
         <v>58.747061983771943</v>
       </c>
-      <c r="S3" s="31">
+      <c r="S3" s="29">
         <f>(0.5*S13*1000*R2^2)/R3</f>
         <v>2.7345613741823587</v>
       </c>
       <c r="T3" s="6"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="36">
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="34">
         <v>0</v>
       </c>
-      <c r="J4" s="37"/>
+      <c r="J4" s="35"/>
       <c r="K4" s="6"/>
-      <c r="L4" s="61" t="s">
+      <c r="L4" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="62"/>
-      <c r="N4" s="62"/>
-      <c r="O4" s="62"/>
-      <c r="P4" s="62"/>
-      <c r="Q4" s="63"/>
-      <c r="R4" s="64">
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="60"/>
+      <c r="P4" s="60"/>
+      <c r="Q4" s="61"/>
+      <c r="R4" s="62">
         <f>4.18*(1-0.0075*I4)</f>
         <v>4.18</v>
       </c>
-      <c r="S4" s="65"/>
+      <c r="S4" s="63"/>
       <c r="T4" s="6"/>
     </row>
-    <row r="5" spans="1:21" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="51" t="s">
+    <row r="5" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="54">
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="52">
         <v>16</v>
       </c>
-      <c r="J5" s="55"/>
+      <c r="J5" s="53"/>
       <c r="K5" s="6"/>
-      <c r="L5" s="61" t="s">
+      <c r="L5" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="62"/>
-      <c r="N5" s="62"/>
-      <c r="O5" s="62"/>
-      <c r="P5" s="62"/>
-      <c r="Q5" s="63"/>
-      <c r="R5" s="64">
+      <c r="M5" s="60"/>
+      <c r="N5" s="60"/>
+      <c r="O5" s="60"/>
+      <c r="P5" s="60"/>
+      <c r="Q5" s="61"/>
+      <c r="R5" s="62">
         <f>I7/(R4*(((I6-I5)^2)^0.5))</f>
         <v>0</v>
       </c>
-      <c r="S5" s="65"/>
+      <c r="S5" s="63"/>
       <c r="T5" s="6"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="56" t="s">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A6" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="59">
+      <c r="B6" s="55"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="57">
         <v>19</v>
       </c>
-      <c r="J6" s="60"/>
+      <c r="J6" s="58"/>
       <c r="K6" s="6"/>
-      <c r="L6" s="66" t="s">
+      <c r="L6" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="M6" s="67"/>
-      <c r="N6" s="67"/>
-      <c r="O6" s="67"/>
-      <c r="P6" s="67"/>
-      <c r="Q6" s="68"/>
-      <c r="R6" s="69" t="str">
+      <c r="M6" s="65"/>
+      <c r="N6" s="65"/>
+      <c r="O6" s="65"/>
+      <c r="P6" s="65"/>
+      <c r="Q6" s="66"/>
+      <c r="R6" s="67" t="str">
         <f>IF(I2&lt;64,IF(R2&gt;0.75,IF(R2&lt;1.5,"Yes",""),""),"")</f>
         <v/>
       </c>
-      <c r="S6" s="70" t="str">
+      <c r="S6" s="68" t="str">
         <f>IF(R6="yes","",IF(R7="yes","","No"))</f>
         <v>No</v>
       </c>
-      <c r="T6" s="19"/>
+      <c r="T6" s="17"/>
       <c r="U6" s="5"/>
     </row>
-    <row r="7" spans="1:21" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="51" t="s">
+    <row r="7" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="52"/>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="54"/>
-      <c r="J7" s="55"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="53"/>
       <c r="K7" s="6"/>
-      <c r="L7" s="71" t="s">
+      <c r="L7" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="72"/>
-      <c r="N7" s="72"/>
-      <c r="O7" s="72"/>
-      <c r="P7" s="72"/>
-      <c r="Q7" s="73"/>
-      <c r="R7" s="74" t="str">
+      <c r="M7" s="70"/>
+      <c r="N7" s="70"/>
+      <c r="O7" s="70"/>
+      <c r="P7" s="70"/>
+      <c r="Q7" s="71"/>
+      <c r="R7" s="72" t="str">
         <f>IF(I2&gt;64,IF(R2&gt;1.25,IF(R2&lt;3,"Yes",""),""),"")</f>
         <v/>
       </c>
-      <c r="S7" s="75"/>
-    </row>
-    <row r="8" spans="1:21" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
+      <c r="S7" s="73"/>
+    </row>
+    <row r="8" spans="1:21" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
       <c r="K8" s="6"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="20"/>
-      <c r="S8" s="20"/>
-    </row>
-    <row r="9" spans="1:21" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="41" t="s">
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="18"/>
+    </row>
+    <row r="9" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="44"/>
-      <c r="M9" s="44"/>
-      <c r="N9" s="44"/>
-      <c r="O9" s="44"/>
-      <c r="P9" s="44"/>
-      <c r="Q9" s="44"/>
-      <c r="R9" s="44"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="str">
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="42"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="42"/>
+      <c r="Q9" s="42"/>
+      <c r="R9" s="42"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A10" s="43" t="str">
         <f>IF(A18&gt;0.75,IF(A18&lt;1.5,"*",""),"")</f>
         <v/>
       </c>
-      <c r="B10" s="46" t="str">
+      <c r="B10" s="44" t="str">
         <f>IF(B18&gt;0.65,IF(B18&lt;1.5,"*",""),"")</f>
         <v/>
       </c>
-      <c r="C10" s="46" t="str">
+      <c r="C10" s="44" t="str">
         <f>IF(C18&gt;0.75,IF(C18&lt;1.5,"*",""),"")</f>
         <v/>
       </c>
-      <c r="D10" s="46" t="str">
+      <c r="D10" s="44" t="str">
         <f>IF(D18&gt;0.75,IF(D18&lt;1.5,"*",""),"")</f>
         <v/>
       </c>
-      <c r="E10" s="46" t="str">
+      <c r="E10" s="44" t="str">
         <f>IF(E18&gt;0.75,IF(E18&lt;1.5,"*",""),"")</f>
         <v/>
       </c>
-      <c r="F10" s="46" t="str">
+      <c r="F10" s="44" t="str">
         <f>IF(F18&gt;0.75,IF(F18&lt;1.5,"*",""),"")</f>
         <v/>
       </c>
-      <c r="G10" s="46" t="str">
+      <c r="G10" s="44" t="str">
         <f>IF(G18&gt;0.75,IF(G18&lt;1.5,"*",""),"")</f>
         <v>*</v>
       </c>
-      <c r="H10" s="46" t="str">
+      <c r="H10" s="44" t="str">
         <f>IF(H18&gt;0.85,IF(H18&lt;3,"*",""),"")</f>
         <v/>
       </c>
-      <c r="I10" s="46" t="str">
+      <c r="I10" s="44" t="str">
         <f t="shared" ref="I10:R10" si="0">IF(I18&gt;1.25,IF(I18&lt;3,"*",""),"")</f>
         <v/>
       </c>
-      <c r="J10" s="46" t="str">
+      <c r="J10" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K10" s="46" t="str">
+      <c r="K10" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="L10" s="46" t="str">
+      <c r="L10" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M10" s="46" t="str">
+      <c r="M10" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="N10" s="46" t="str">
+      <c r="N10" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="O10" s="46" t="str">
+      <c r="O10" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P10" s="46" t="str">
+      <c r="P10" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="Q10" s="46" t="str">
+      <c r="Q10" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="R10" s="47" t="str">
+      <c r="R10" s="45" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="48">
+    <row r="11" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="46">
         <v>10</v>
       </c>
-      <c r="B11" s="49">
+      <c r="B11" s="47">
         <v>15</v>
       </c>
-      <c r="C11" s="49">
+      <c r="C11" s="47">
         <v>20</v>
       </c>
-      <c r="D11" s="49">
+      <c r="D11" s="47">
         <v>25</v>
       </c>
-      <c r="E11" s="49">
+      <c r="E11" s="47">
         <v>32</v>
       </c>
-      <c r="F11" s="49">
+      <c r="F11" s="47">
         <v>40</v>
       </c>
-      <c r="G11" s="49">
+      <c r="G11" s="47">
         <v>50</v>
       </c>
-      <c r="H11" s="49">
+      <c r="H11" s="47">
         <v>65</v>
       </c>
-      <c r="I11" s="49">
+      <c r="I11" s="47">
         <v>80</v>
       </c>
-      <c r="J11" s="49">
+      <c r="J11" s="47">
         <v>100</v>
       </c>
-      <c r="K11" s="49">
+      <c r="K11" s="47">
         <v>150</v>
       </c>
-      <c r="L11" s="49">
+      <c r="L11" s="47">
         <v>200</v>
       </c>
-      <c r="M11" s="49">
+      <c r="M11" s="47">
         <v>250</v>
       </c>
-      <c r="N11" s="49">
+      <c r="N11" s="47">
         <v>300</v>
       </c>
-      <c r="O11" s="49">
+      <c r="O11" s="47">
         <v>350</v>
       </c>
-      <c r="P11" s="49">
+      <c r="P11" s="47">
         <v>400</v>
       </c>
-      <c r="Q11" s="49">
+      <c r="Q11" s="47">
         <v>450</v>
       </c>
-      <c r="R11" s="50">
+      <c r="R11" s="48">
         <v>600</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -1674,12 +1690,12 @@
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
       <c r="I13" s="11"/>
-      <c r="J13" s="14">
+      <c r="J13" s="76">
         <f>((R2*S15*(1000*S13))/J15)*1000</f>
         <v>34681.646591334807</v>
       </c>
-      <c r="K13" s="15"/>
-      <c r="L13" s="16"/>
+      <c r="K13" s="77"/>
+      <c r="L13" s="78"/>
       <c r="M13" s="9" t="s">
         <v>16</v>
       </c>
@@ -1695,7 +1711,7 @@
       <c r="T13" s="12"/>
       <c r="U13" s="6"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>17</v>
       </c>
@@ -1707,12 +1723,12 @@
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
       <c r="I14" s="11"/>
-      <c r="J14" s="17">
+      <c r="J14" s="81">
         <f>(309*((1-EXP(-0.111*(37+I5)))/(37+I5))^1.42)*EXP(1.1*I4*(256-I5)*10^-4)</f>
         <v>1.0958874917403498</v>
       </c>
-      <c r="K14" s="15"/>
-      <c r="L14" s="11"/>
+      <c r="K14" s="82"/>
+      <c r="L14" s="83"/>
       <c r="M14" s="9" t="s">
         <v>18</v>
       </c>
@@ -1721,14 +1737,14 @@
       <c r="P14" s="10"/>
       <c r="Q14" s="10"/>
       <c r="R14" s="11"/>
-      <c r="S14" s="12">
+      <c r="S14" s="79">
         <f>J16/S15</f>
         <v>6.8656716417910446E-4</v>
       </c>
-      <c r="T14" s="12"/>
+      <c r="T14" s="80"/>
       <c r="U14" s="6"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>19</v>
       </c>
@@ -1761,7 +1777,7 @@
       <c r="T15" s="12"/>
       <c r="U15" s="6"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>21</v>
       </c>
@@ -1773,14 +1789,14 @@
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
       <c r="I16" s="11"/>
-      <c r="J16" s="18">
+      <c r="J16" s="16">
         <f>IF(I1="HG BMS",data!B10,IF(I1 ="MG BMS",data!B11,IF(I1="GMS",data!B12,IF(I1="Cu",data!B13,IF(I1="Other",data!B14,"error")))))</f>
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="K16" s="15"/>
       <c r="L16" s="11"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <f t="shared" ref="A18:J18" si="1">($I$3/1000)/(3.14159*(A11/2000)^2)</f>
         <v>25.464812403910123</v>
@@ -1854,106 +1870,109 @@
         <v>7.073559001086146E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
       <c r="T22" s="4"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="Q23" s="5"/>
       <c r="T23" s="4"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="T24" s="4"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="8"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="T25" s="4"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="8"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="T26" s="4"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="8"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="T27" s="4"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="T28" s="4"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="8"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="T29" s="4"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="8"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="T30" s="4"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="8"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="T31" s="4"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="T32" s="4"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="T33" s="4"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="T34" s="4"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="T35" s="4"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="T36" s="4"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="T37" s="4"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="T38" s="4"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" s="8"/>
       <c r="N39" s="5"/>
       <c r="O39" s="5"/>
       <c r="T39" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="I3:J3"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="J14:L14"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
@@ -1969,7 +1988,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
@@ -1987,7 +2006,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
@@ -2005,7 +2024,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
@@ -2023,7 +2042,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
@@ -2041,7 +2060,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
@@ -2059,7 +2078,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
@@ -2075,16 +2094,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B14"/>
+    <sheetView topLeftCell="A10" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.36328125" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -2143,12 +2162,12 @@
         <v>600</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -2207,7 +2226,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>25</v>
       </c>
@@ -2266,7 +2285,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
@@ -2326,7 +2345,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -2385,7 +2404,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>29</v>
       </c>
@@ -2444,12 +2463,12 @@
         <v>590</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
@@ -2457,7 +2476,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>25</v>
       </c>
@@ -2465,7 +2484,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
@@ -2473,7 +2492,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
@@ -2481,7 +2500,7 @@
         <v>1.5E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>29</v>
       </c>
@@ -2489,7 +2508,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -2504,7 +2523,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -2519,7 +2538,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -2534,7 +2553,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -2549,7 +2568,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -2565,7 +2584,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2582,7 +2600,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
@@ -2600,7 +2618,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
@@ -2618,7 +2636,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
@@ -2636,7 +2654,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
@@ -2654,7 +2672,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
@@ -2672,7 +2690,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
@@ -2690,7 +2708,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>

</xml_diff>